<commit_message>
Enhance timetable generation scripts by adding room name to room number mapping functionality and updating group mappings to include music instrument prefixes. Introduce debug logging for better traceability during processing. Update CSV files to reflect changes in room naming conventions and group mappings.
</commit_message>
<xml_diff>
--- a/student_timetables/Cybi CHENG_CampA_timetable.xlsx
+++ b/student_timetables/Cybi CHENG_CampA_timetable.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Full Timetable" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Full Timetable" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -591,7 +591,7 @@
       <c r="D7" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Ivy CHUANG 
-(Room Ivy)</t>
+(Room G14)</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
@@ -603,7 +603,7 @@
       <c r="F7" s="1" t="inlineStr">
         <is>
           <t>Flute MasterClass
-(Room Stephane)</t>
+(Room G19)</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
@@ -661,13 +661,13 @@
       <c r="C11" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Ivy CHUANG 
-(Room Ivy)</t>
+(Room G14)</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
           <t>Rehearsal with pianist
-(Room Shelley)</t>
+(Room G22)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -799,7 +799,7 @@
       <c r="B19" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Stephane RETY 
-(Room Stephane)</t>
+(Room G19)</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
@@ -817,13 +817,13 @@
       <c r="E19" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Stephane RETY &amp; pianist 
-(Room Stephane)</t>
+(Room G19)</t>
         </is>
       </c>
       <c r="F19" s="1" t="inlineStr">
         <is>
           <t>Flute MasterClass
-(Room Stephane)</t>
+(Room G19)</t>
         </is>
       </c>
       <c r="G19" s="1" t="n"/>
@@ -961,31 +961,31 @@
       <c r="B27" s="1" t="inlineStr">
         <is>
           <t>Ensemble 
-(Room Tomasz)</t>
+(Room G15)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
           <t>Ensemble 
-(Room Tomasz)</t>
+(Room G15)</t>
         </is>
       </c>
       <c r="D27" s="1" t="inlineStr">
         <is>
           <t>Ensemble 
-(Room Tomasz)</t>
+(Room G15)</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
           <t>Ensemble 
-(Room Tomasz)</t>
+(Room G15)</t>
         </is>
       </c>
       <c r="F27" s="1" t="inlineStr">
         <is>
           <t>Ensemble 
-(Room Tomasz)</t>
+(Room G15)</t>
         </is>
       </c>
       <c r="G27" s="1" t="inlineStr">

</xml_diff>